<commit_message>
moving execution to condor
</commit_message>
<xml_diff>
--- a/data/Hika.xlsx
+++ b/data/Hika.xlsx
@@ -905,8 +905,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1251,12 +1251,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EE101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="2"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -1663,7 +1668,7 @@
       </c>
     </row>
     <row r="2" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+      <c r="A2" s="2">
         <v>40338.371527777781</v>
       </c>
       <c r="B2">
@@ -2070,7 +2075,7 @@
       </c>
     </row>
     <row r="3" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+      <c r="A3" s="2">
         <v>40339.375</v>
       </c>
       <c r="B3">
@@ -2477,7 +2482,7 @@
       </c>
     </row>
     <row r="4" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="A4" s="2">
         <v>40343.375</v>
       </c>
       <c r="B4">
@@ -2884,7 +2889,7 @@
       </c>
     </row>
     <row r="5" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="A5" s="2">
         <v>40344.368055555555</v>
       </c>
       <c r="B5">
@@ -3291,7 +3296,7 @@
       </c>
     </row>
     <row r="6" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+      <c r="A6" s="2">
         <v>40345.371527777781</v>
       </c>
       <c r="B6">
@@ -3698,7 +3703,7 @@
       </c>
     </row>
     <row r="7" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+      <c r="A7" s="2">
         <v>40346.371527777781</v>
       </c>
       <c r="B7">
@@ -4105,7 +4110,7 @@
       </c>
     </row>
     <row r="8" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+      <c r="A8" s="2">
         <v>40350.375</v>
       </c>
       <c r="B8">
@@ -4512,7 +4517,7 @@
       </c>
     </row>
     <row r="9" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+      <c r="A9" s="2">
         <v>40351.458333333336</v>
       </c>
       <c r="B9">
@@ -4919,7 +4924,7 @@
       </c>
     </row>
     <row r="10" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+      <c r="A10" s="2">
         <v>40352.4375</v>
       </c>
       <c r="B10">
@@ -5326,7 +5331,7 @@
       </c>
     </row>
     <row r="11" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+      <c r="A11" s="2">
         <v>40353.364583333336</v>
       </c>
       <c r="B11">
@@ -5733,7 +5738,7 @@
       </c>
     </row>
     <row r="12" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+      <c r="A12" s="2">
         <v>40357.375</v>
       </c>
       <c r="B12">
@@ -6140,7 +6145,7 @@
       </c>
     </row>
     <row r="13" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+      <c r="A13" s="2">
         <v>40358.368055555555</v>
       </c>
       <c r="B13">
@@ -6377,7 +6382,7 @@
       <c r="CA13">
         <v>-2.2720890000000001E-3</v>
       </c>
-      <c r="CB13" s="2">
+      <c r="CB13" s="1">
         <v>8.1199999999999995E-5</v>
       </c>
       <c r="CC13">
@@ -6547,7 +6552,7 @@
       </c>
     </row>
     <row r="14" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+      <c r="A14" s="2">
         <v>40359.364583333336</v>
       </c>
       <c r="B14">
@@ -6954,7 +6959,7 @@
       </c>
     </row>
     <row r="15" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+      <c r="A15" s="2">
         <v>40360.375</v>
       </c>
       <c r="B15">
@@ -7361,7 +7366,7 @@
       </c>
     </row>
     <row r="16" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
+      <c r="A16" s="2">
         <v>40365.381944444445</v>
       </c>
       <c r="B16">
@@ -7768,7 +7773,7 @@
       </c>
     </row>
     <row r="17" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
+      <c r="A17" s="2">
         <v>40366.354166666664</v>
       </c>
       <c r="B17">
@@ -8175,7 +8180,7 @@
       </c>
     </row>
     <row r="18" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
+      <c r="A18" s="2">
         <v>40367.357638888891</v>
       </c>
       <c r="B18">
@@ -8582,7 +8587,7 @@
       </c>
     </row>
     <row r="19" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
+      <c r="A19" s="2">
         <v>40371.34375</v>
       </c>
       <c r="B19">
@@ -8989,7 +8994,7 @@
       </c>
     </row>
     <row r="20" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
+      <c r="A20" s="2">
         <v>40372.34375</v>
       </c>
       <c r="B20">
@@ -9396,7 +9401,7 @@
       </c>
     </row>
     <row r="21" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
+      <c r="A21" s="2">
         <v>40373.350694444445</v>
       </c>
       <c r="B21">
@@ -9803,7 +9808,7 @@
       </c>
     </row>
     <row r="22" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
+      <c r="A22" s="2">
         <v>40374.347222222219</v>
       </c>
       <c r="B22">
@@ -10210,7 +10215,7 @@
       </c>
     </row>
     <row r="23" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
+      <c r="A23" s="2">
         <v>40378.34375</v>
       </c>
       <c r="B23">
@@ -10617,7 +10622,7 @@
       </c>
     </row>
     <row r="24" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
+      <c r="A24" s="2">
         <v>40379.354166666664</v>
       </c>
       <c r="B24">
@@ -11024,7 +11029,7 @@
       </c>
     </row>
     <row r="25" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
+      <c r="A25" s="2">
         <v>40380.357638888891</v>
       </c>
       <c r="B25">
@@ -11288,7 +11293,7 @@
       <c r="CJ25">
         <v>1.143271E-3</v>
       </c>
-      <c r="CK25" s="2">
+      <c r="CK25" s="1">
         <v>-1.88E-5</v>
       </c>
       <c r="CL25">
@@ -11431,7 +11436,7 @@
       </c>
     </row>
     <row r="26" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
+      <c r="A26" s="2">
         <v>40381.354166666664</v>
       </c>
       <c r="B26">
@@ -11838,7 +11843,7 @@
       </c>
     </row>
     <row r="27" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
+      <c r="A27" s="2">
         <v>40385.354166666664</v>
       </c>
       <c r="B27">
@@ -12245,7 +12250,7 @@
       </c>
     </row>
     <row r="28" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
+      <c r="A28" s="2">
         <v>40386.354166666664</v>
       </c>
       <c r="B28">
@@ -12652,7 +12657,7 @@
       </c>
     </row>
     <row r="29" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
+      <c r="A29" s="2">
         <v>40387.354166666664</v>
       </c>
       <c r="B29">
@@ -13059,7 +13064,7 @@
       </c>
     </row>
     <row r="30" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
+      <c r="A30" s="2">
         <v>40388.354166666664</v>
       </c>
       <c r="B30">
@@ -13466,7 +13471,7 @@
       </c>
     </row>
     <row r="31" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
+      <c r="A31" s="2">
         <v>40392.354166666664</v>
       </c>
       <c r="B31">
@@ -13873,7 +13878,7 @@
       </c>
     </row>
     <row r="32" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
+      <c r="A32" s="2">
         <v>40393.354166666664</v>
       </c>
       <c r="B32">
@@ -14280,7 +14285,7 @@
       </c>
     </row>
     <row r="33" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
+      <c r="A33" s="2">
         <v>40394.354166666664</v>
       </c>
       <c r="B33">
@@ -14687,7 +14692,7 @@
       </c>
     </row>
     <row r="34" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
+      <c r="A34" s="2">
         <v>40395.354166666664</v>
       </c>
       <c r="B34">
@@ -15094,7 +15099,7 @@
       </c>
     </row>
     <row r="35" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
+      <c r="A35" s="2">
         <v>40399.270833333336</v>
       </c>
       <c r="B35">
@@ -15501,7 +15506,7 @@
       </c>
     </row>
     <row r="36" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
+      <c r="A36" s="2">
         <v>40400.260416666664</v>
       </c>
       <c r="B36">
@@ -15908,7 +15913,7 @@
       </c>
     </row>
     <row r="37" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
+      <c r="A37" s="2">
         <v>40401.263888888891</v>
       </c>
       <c r="B37">
@@ -16315,7 +16320,7 @@
       </c>
     </row>
     <row r="38" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
+      <c r="A38" s="2">
         <v>40402.390972222223</v>
       </c>
       <c r="B38">
@@ -16722,7 +16727,7 @@
       </c>
     </row>
     <row r="39" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
+      <c r="A39" s="2">
         <v>40406.263888888891</v>
       </c>
       <c r="B39">
@@ -17129,7 +17134,7 @@
       </c>
     </row>
     <row r="40" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
+      <c r="A40" s="2">
         <v>40407.260416666664</v>
       </c>
       <c r="B40">
@@ -17536,7 +17541,7 @@
       </c>
     </row>
     <row r="41" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
+      <c r="A41" s="2">
         <v>40408.246527777781</v>
       </c>
       <c r="B41">
@@ -17943,7 +17948,7 @@
       </c>
     </row>
     <row r="42" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
+      <c r="A42" s="2">
         <v>40409.354166666664</v>
       </c>
       <c r="B42">
@@ -18350,7 +18355,7 @@
       </c>
     </row>
     <row r="43" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
+      <c r="A43" s="2">
         <v>40413.25</v>
       </c>
       <c r="B43">
@@ -18757,7 +18762,7 @@
       </c>
     </row>
     <row r="44" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A44" s="1">
+      <c r="A44" s="2">
         <v>40414.246527777781</v>
       </c>
       <c r="B44">
@@ -19164,7 +19169,7 @@
       </c>
     </row>
     <row r="45" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
+      <c r="A45" s="2">
         <v>40415.25</v>
       </c>
       <c r="B45">
@@ -19571,7 +19576,7 @@
       </c>
     </row>
     <row r="46" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
+      <c r="A46" s="2">
         <v>40416.25</v>
       </c>
       <c r="B46">
@@ -19978,7 +19983,7 @@
       </c>
     </row>
     <row r="47" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A47" s="1">
+      <c r="A47" s="2">
         <v>40694.597222222219</v>
       </c>
       <c r="B47">
@@ -20385,7 +20390,7 @@
       </c>
     </row>
     <row r="48" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A48" s="1">
+      <c r="A48" s="2">
         <v>40697.555555555555</v>
       </c>
       <c r="B48">
@@ -20792,7 +20797,7 @@
       </c>
     </row>
     <row r="49" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
+      <c r="A49" s="2">
         <v>40700.447916666664</v>
       </c>
       <c r="B49">
@@ -21199,7 +21204,7 @@
       </c>
     </row>
     <row r="50" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A50" s="1">
+      <c r="A50" s="2">
         <v>40702.395833333336</v>
       </c>
       <c r="B50">
@@ -21606,7 +21611,7 @@
       </c>
     </row>
     <row r="51" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A51" s="1">
+      <c r="A51" s="2">
         <v>40707.381944444445</v>
       </c>
       <c r="B51">
@@ -22013,7 +22018,7 @@
       </c>
     </row>
     <row r="52" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A52" s="1">
+      <c r="A52" s="2">
         <v>40708.385416666664</v>
       </c>
       <c r="B52">
@@ -22420,7 +22425,7 @@
       </c>
     </row>
     <row r="53" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A53" s="1">
+      <c r="A53" s="2">
         <v>40710.527777777781</v>
       </c>
       <c r="B53">
@@ -22827,7 +22832,7 @@
       </c>
     </row>
     <row r="54" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A54" s="1">
+      <c r="A54" s="2">
         <v>40714.375694444447</v>
       </c>
       <c r="B54">
@@ -23234,7 +23239,7 @@
       </c>
     </row>
     <row r="55" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A55" s="1">
+      <c r="A55" s="2">
         <v>40715.399305555555</v>
       </c>
       <c r="B55">
@@ -23641,7 +23646,7 @@
       </c>
     </row>
     <row r="56" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A56" s="1">
+      <c r="A56" s="2">
         <v>40716.379861111112</v>
       </c>
       <c r="B56">
@@ -24048,7 +24053,7 @@
       </c>
     </row>
     <row r="57" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A57" s="1">
+      <c r="A57" s="2">
         <v>40717.5625</v>
       </c>
       <c r="B57">
@@ -24455,7 +24460,7 @@
       </c>
     </row>
     <row r="58" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A58" s="1">
+      <c r="A58" s="2">
         <v>40720.65625</v>
       </c>
       <c r="B58">
@@ -24862,7 +24867,7 @@
       </c>
     </row>
     <row r="59" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A59" s="1">
+      <c r="A59" s="2">
         <v>40721.481249999997</v>
       </c>
       <c r="B59">
@@ -25269,7 +25274,7 @@
       </c>
     </row>
     <row r="60" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A60" s="1">
+      <c r="A60" s="2">
         <v>40722.385416666664</v>
       </c>
       <c r="B60">
@@ -25676,7 +25681,7 @@
       </c>
     </row>
     <row r="61" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A61" s="1">
+      <c r="A61" s="2">
         <v>40723.397916666669</v>
       </c>
       <c r="B61">
@@ -26083,7 +26088,7 @@
       </c>
     </row>
     <row r="62" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A62" s="1">
+      <c r="A62" s="2">
         <v>40729.392361111109</v>
       </c>
       <c r="B62">
@@ -26490,7 +26495,7 @@
       </c>
     </row>
     <row r="63" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A63" s="1">
+      <c r="A63" s="2">
         <v>40730.377083333333</v>
       </c>
       <c r="B63">
@@ -26897,7 +26902,7 @@
       </c>
     </row>
     <row r="64" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A64" s="1">
+      <c r="A64" s="2">
         <v>40731.378472222219</v>
       </c>
       <c r="B64">
@@ -27304,7 +27309,7 @@
       </c>
     </row>
     <row r="65" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A65" s="1">
+      <c r="A65" s="2">
         <v>40732.524305555555</v>
       </c>
       <c r="B65">
@@ -27711,7 +27716,7 @@
       </c>
     </row>
     <row r="66" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A66" s="1">
+      <c r="A66" s="2">
         <v>40735.378472222219</v>
       </c>
       <c r="B66">
@@ -28118,7 +28123,7 @@
       </c>
     </row>
     <row r="67" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A67" s="1">
+      <c r="A67" s="2">
         <v>40736.378472222219</v>
       </c>
       <c r="B67">
@@ -28525,7 +28530,7 @@
       </c>
     </row>
     <row r="68" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A68" s="1">
+      <c r="A68" s="2">
         <v>40738.378472222219</v>
       </c>
       <c r="B68">
@@ -28932,7 +28937,7 @@
       </c>
     </row>
     <row r="69" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A69" s="1">
+      <c r="A69" s="2">
         <v>40742.392361111109</v>
       </c>
       <c r="B69">
@@ -29339,7 +29344,7 @@
       </c>
     </row>
     <row r="70" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A70" s="1">
+      <c r="A70" s="2">
         <v>40743.388888888891</v>
       </c>
       <c r="B70">
@@ -29746,7 +29751,7 @@
       </c>
     </row>
     <row r="71" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A71" s="1">
+      <c r="A71" s="2">
         <v>40744.382638888892</v>
       </c>
       <c r="B71">
@@ -30153,7 +30158,7 @@
       </c>
     </row>
     <row r="72" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A72" s="1">
+      <c r="A72" s="2">
         <v>40745.40625</v>
       </c>
       <c r="B72">
@@ -30560,7 +30565,7 @@
       </c>
     </row>
     <row r="73" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A73" s="1">
+      <c r="A73" s="2">
         <v>40749.484027777777</v>
       </c>
       <c r="B73">
@@ -30967,7 +30972,7 @@
       </c>
     </row>
     <row r="74" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A74" s="1">
+      <c r="A74" s="2">
         <v>40750.402083333334</v>
       </c>
       <c r="B74">
@@ -31374,7 +31379,7 @@
       </c>
     </row>
     <row r="75" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A75" s="1">
+      <c r="A75" s="2">
         <v>40751.392361111109</v>
       </c>
       <c r="B75">
@@ -31781,7 +31786,7 @@
       </c>
     </row>
     <row r="76" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A76" s="1">
+      <c r="A76" s="2">
         <v>40752.396527777775</v>
       </c>
       <c r="B76">
@@ -32188,7 +32193,7 @@
       </c>
     </row>
     <row r="77" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A77" s="1">
+      <c r="A77" s="2">
         <v>40756.401388888888</v>
       </c>
       <c r="B77">
@@ -32595,7 +32600,7 @@
       </c>
     </row>
     <row r="78" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A78" s="1">
+      <c r="A78" s="2">
         <v>40757.392361111109</v>
       </c>
       <c r="B78">
@@ -33002,7 +33007,7 @@
       </c>
     </row>
     <row r="79" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A79" s="1">
+      <c r="A79" s="2">
         <v>40758.387499999997</v>
       </c>
       <c r="B79">
@@ -33409,7 +33414,7 @@
       </c>
     </row>
     <row r="80" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A80" s="1">
+      <c r="A80" s="2">
         <v>40763.404166666667</v>
       </c>
       <c r="B80">
@@ -33816,7 +33821,7 @@
       </c>
     </row>
     <row r="81" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A81" s="1">
+      <c r="A81" s="2">
         <v>40764.385416666664</v>
       </c>
       <c r="B81">
@@ -34223,7 +34228,7 @@
       </c>
     </row>
     <row r="82" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A82" s="1">
+      <c r="A82" s="2">
         <v>40765.399305555555</v>
       </c>
       <c r="B82">
@@ -34630,7 +34635,7 @@
       </c>
     </row>
     <row r="83" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A83" s="1">
+      <c r="A83" s="2">
         <v>40766.489583333336</v>
       </c>
       <c r="B83">
@@ -35037,7 +35042,7 @@
       </c>
     </row>
     <row r="84" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A84" s="1">
+      <c r="A84" s="2">
         <v>40770.378472222219</v>
       </c>
       <c r="B84">
@@ -35444,7 +35449,7 @@
       </c>
     </row>
     <row r="85" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A85" s="1">
+      <c r="A85" s="2">
         <v>40771.385416666664</v>
       </c>
       <c r="B85">
@@ -35851,7 +35856,7 @@
       </c>
     </row>
     <row r="86" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A86" s="1">
+      <c r="A86" s="2">
         <v>40772.399305555555</v>
       </c>
       <c r="B86">
@@ -36258,7 +36263,7 @@
       </c>
     </row>
     <row r="87" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A87" s="1">
+      <c r="A87" s="2">
         <v>40775.513888888891</v>
       </c>
       <c r="B87">
@@ -36665,7 +36670,7 @@
       </c>
     </row>
     <row r="88" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A88" s="1">
+      <c r="A88" s="2">
         <v>40776.538194444445</v>
       </c>
       <c r="B88">
@@ -37072,7 +37077,7 @@
       </c>
     </row>
     <row r="89" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A89" s="1">
+      <c r="A89" s="2">
         <v>40777.336805555555</v>
       </c>
       <c r="B89">
@@ -37479,7 +37484,7 @@
       </c>
     </row>
     <row r="90" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A90" s="1">
+      <c r="A90" s="2">
         <v>40782.451388888891</v>
       </c>
       <c r="B90">
@@ -37886,7 +37891,7 @@
       </c>
     </row>
     <row r="91" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A91" s="1">
+      <c r="A91" s="2">
         <v>40783.563888888886</v>
       </c>
       <c r="B91">
@@ -38293,7 +38298,7 @@
       </c>
     </row>
     <row r="92" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A92" s="1">
+      <c r="A92" s="2">
         <v>40784.515277777777</v>
       </c>
       <c r="B92">
@@ -38700,7 +38705,7 @@
       </c>
     </row>
     <row r="93" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A93" s="1">
+      <c r="A93" s="2">
         <v>40785.338888888888</v>
       </c>
       <c r="B93">
@@ -39107,7 +39112,7 @@
       </c>
     </row>
     <row r="94" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A94" s="1">
+      <c r="A94" s="2">
         <v>41057.506249999999</v>
       </c>
       <c r="B94">
@@ -39514,7 +39519,7 @@
       </c>
     </row>
     <row r="95" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A95" s="1">
+      <c r="A95" s="2">
         <v>41058.423611111109</v>
       </c>
       <c r="B95">
@@ -39544,7 +39549,7 @@
       <c r="J95">
         <v>0</v>
       </c>
-      <c r="K95" s="2">
+      <c r="K95" s="1">
         <v>4.7200000000000002E-5</v>
       </c>
       <c r="L95">
@@ -39921,7 +39926,7 @@
       </c>
     </row>
     <row r="96" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A96" s="1">
+      <c r="A96" s="2">
         <v>41060.465277777781</v>
       </c>
       <c r="B96">
@@ -40328,7 +40333,7 @@
       </c>
     </row>
     <row r="97" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A97" s="1">
+      <c r="A97" s="2">
         <v>41061.458333333336</v>
       </c>
       <c r="B97">
@@ -40735,7 +40740,7 @@
       </c>
     </row>
     <row r="98" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A98" s="1">
+      <c r="A98" s="2">
         <v>41064.427777777775</v>
       </c>
       <c r="B98">
@@ -41142,7 +41147,7 @@
       </c>
     </row>
     <row r="99" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A99" s="1">
+      <c r="A99" s="2">
         <v>41065.396527777775</v>
       </c>
       <c r="B99">
@@ -41549,7 +41554,7 @@
       </c>
     </row>
     <row r="100" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A100" s="1">
+      <c r="A100" s="2">
         <v>41066.397222222222</v>
       </c>
       <c r="B100">
@@ -41582,7 +41587,7 @@
       <c r="K100">
         <v>0</v>
       </c>
-      <c r="L100" s="2">
+      <c r="L100" s="1">
         <v>6.4499999999999996E-5</v>
       </c>
       <c r="M100">
@@ -41956,7 +41961,7 @@
       </c>
     </row>
     <row r="101" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A101" s="1">
+      <c r="A101" s="2">
         <v>41067.404166666667</v>
       </c>
       <c r="B101">
@@ -42364,5 +42369,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>